<commit_message>
Subiendo mas experimentos realizados
</commit_message>
<xml_diff>
--- a/modelos/Resultados Experimentos.xlsx
+++ b/modelos/Resultados Experimentos.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>N°</t>
   </si>
@@ -100,14 +100,6 @@
     </r>
   </si>
   <si>
-    <t>• Preprocesamiento del modelo base.
-• Entrenamos el modelo con valores aleatorios 150 veces usando previamente la técnica RandomizedSearchCV (cv=5, n_iter=30).</t>
-  </si>
-  <si>
-    <t>• Preprocesamiento del modelo base.
-• Entrenamos el modelo con valores aleatorios 300 veces usando previamente la técnica RandomizedSearchCV (cv=10, n_iter=30).</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">{'bootstrap': False,
  'criterion': 'gini',
@@ -200,9 +192,6 @@
     <t>Experimiento_002_Proyecto_ML_Random_Forest.ipynb</t>
   </si>
   <si>
-    <t>Experimiento_003_Proyecto_ML_SVM.ipynb</t>
-  </si>
-  <si>
     <t>Responsable</t>
   </si>
   <si>
@@ -210,6 +199,455 @@
   </si>
   <si>
     <t>Parámetros Entrenamiento</t>
+  </si>
+  <si>
+    <t>SVC(kernel='linear', C=20)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Tipo kernel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+• Asignamos C=20.</t>
+    </r>
+  </si>
+  <si>
+    <t>SVC(kernel='linear', C=100)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Tipo kernel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Linear</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+• Asignamos C=100.</t>
+    </r>
+  </si>
+  <si>
+    <t>SVC(kernel='rbf', C=3.1623,gamma=0.1000)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Tipo kernel </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Gausiano</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+• Asignamos C=3.1623.
+• Asignamos gamma=0.1000.</t>
+    </r>
+  </si>
+  <si>
+    <t>Experimiento_006_Proyecto_ML_SVM_Gausiano.ipynb</t>
+  </si>
+  <si>
+    <t>Experimiento_005_Proyecto_ML_SVM_Lineal.ipynb</t>
+  </si>
+  <si>
+    <t>Experimiento_004_Proyecto_ML_SVM_Lineal.ipynb</t>
+  </si>
+  <si>
+    <t>Experimiento_003_Proyecto_ML_SVM_Lineal.ipynb</t>
+  </si>
+  <si>
+    <t>Experimiento_007_Proyecto_ML_Random_Forest.ipynb</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{'bootstrap': False,
+ 'criterion': 'gini',
+ 'max_depth': </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">,
+ 'min_samples_leaf': 1,
+ 'min_samples_split': 5,
+ 'n_estimators': </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2152</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Entrenamos el modelo con valores aleatorios 150 veces usando previamente la técnica de búsqueda aleatoria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RandomizedSearchCV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cv=5, n_iter=30).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Entrenamos el modelo con valores aleatorios 300 veces usando previamente la técnica de búsqueda aleatoria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RandomizedSearchCV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cv=10, n_iter=30).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Entrenamos el modelo con valores aleatorios 600 veces usando previamente la técnica de búsqueda aleatoria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RandomizedSearchCV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cv=15, n_iter=40).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">• Preprocesamiento del modelo base.
+• Entrenamos el modelo con valores aleatorios 26400 veces usando previamente la técnica de búsqueda aleatoria </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GridSearchCV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cv=10).</t>
+    </r>
+  </si>
+  <si>
+    <t>Ensamble - VotingClassifier</t>
+  </si>
+  <si>
+    <t>clf1 = DecisionTreeClassifier(max_depth=4)
+clf2 = KNeighborsClassifier(n_neighbors=7)
+clf3 = SVC(gamma=.1, kernel='rbf', probability=True)
+eclf = VotingClassifier(estimators=[('dt', clf1), ('knn', clf2), ('svc', clf3)],voting='soft', weights=[2, 1, 2])</t>
+  </si>
+  <si>
+    <t>Experimiento_008_Proyecto_ML_Ensamble_Voting.ipynb</t>
+  </si>
+  <si>
+    <t>clf1 = RandomForestClassifier(bootstrap=False,criterion='gini',max_depth=200,
+           min_samples_leaf=1,min_samples_split=5,n_estimators=2152)
+clf2 = DecisionTreeClassifier(max_depth=30)
+clf3 = KNeighborsClassifier(n_neighbors=20)
+clf4 = SVC(C=3.1623, gamma=0.1000, kernel='rbf', probability=True)
+eclf = VotingClassifier(estimators=[('rf', clf1),('dt', clf2), ('knn', clf3), ('svc', clf4)],
+          voting='soft', weights=[2, 1, 1, 2])</t>
+  </si>
+  <si>
+    <t>Experimiento_009_Proyecto_ML_Ensamble_Voting.ipynb</t>
+  </si>
+  <si>
+    <t>Ensamble - StackingClassifier</t>
+  </si>
+  <si>
+    <t>• Preprocesamiento del modelo base.
+• Entrenamos con el modelo de ensamble por votación:
+  - DecisionTreeClassifier
+  - KNeighborsClassifier
+  - SVM</t>
+  </si>
+  <si>
+    <t>• Preprocesamiento del modelo base.
+• Entrenamos con el modelo de ensamble por votación:
+  - RandomForest 
+  - DecisionTreeClassifier
+  - KNeighborsClassifier
+  - SVM</t>
+  </si>
+  <si>
+    <t>• Preprocesamiento del modelo base.
+• Entrenamos con el modelo de ensamble por apilamiento:
+  - DecisionTreeClassifier
+  - KNeighborsClassifier
+  - SVM
+• El estimador final es Regresión Logística.</t>
+  </si>
+  <si>
+    <t>Experimiento_010_Proyecto_ML_Ensamble_Stacking.ipynb</t>
+  </si>
+  <si>
+    <r>
+      <t>estimators = [
+     ('árbol de decisión', DecisionTreeClassifier(max_depth=4)),
+     ('k-NN', make_pipeline(StandardScaler(),KNeighborsClassifier(n_neighbors=7) )),
+     ('SVM de kernel gaussiano', make_pipeline(StandardScaler(),
+                                               SVC(kernel='rbf', probability=True) ))
+]
+StackingClassifier(estimators=estimators, 
+                              final_estimator=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogisticRegression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(penalty='l2')</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>estimators = [
+     ('Random Forest', RandomForestClassifier(bootstrap=False,criterion='gini',max_depth=200,
+           min_samples_leaf=1,min_samples_split=5,n_estimators=2152)),
+     ('árbol de decisión', DecisionTreeClassifier(max_depth=50)),
+     ('k-NN', make_pipeline(StandardScaler(),KNeighborsClassifier(n_neighbors=50) )),
+     ('SVM de kernel gaussiano', make_pipeline(StandardScaler(),
+                                               SVC(C=3.1623, gamma=0.1000, kernel='rbf', probability=True) ))
+]
+StackingClassifier(estimators=estimators, 
+                              final_estimator=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LogisticRegression</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(penalty='l2')</t>
+    </r>
+  </si>
+  <si>
+    <t>• Preprocesamiento del modelo base.
+• Entrenamos con el modelo de ensamble por apilamiento:
+  - RandomForest 
+  - DecisionTreeClassifier
+  - KNeighborsClassifier
+  - SVM
+• El estimador final es Regresión Logística.</t>
+  </si>
+  <si>
+    <t>Experimiento_011_Proyecto_ML_Ensamble_Stacking.ipynb</t>
+  </si>
+  <si>
+    <r>
+      <t>estimators = [
+     ('Random Forest', RandomForestClassifier(bootstrap=False,criterion='gini',max_depth=200,
+           min_samples_leaf=1,min_samples_split=5,n_estimators=2152)),
+     ('árbol de decisión', DecisionTreeClassifier(max_depth=50)),
+     ('k-NN', make_pipeline(StandardScaler(),KNeighborsClassifier(n_neighbors=50) )),
+     ('SVM de kernel gaussiano', make_pipeline(StandardScaler(),
+                                               SVC(C=3.1623, gamma=0.1000, kernel='rbf', probability=True) ))
+]
+StackingClassifier(estimators=estimators, 
+                              final_estimator=</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RandomForestClassifier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>• Preprocesamiento del modelo base.
+• Entrenamos con el modelo de ensamble por apilamiento:
+  - RandomForest 
+  - DecisionTreeClassifier
+  - KNeighborsClassifier
+  - SVM
+• El estimador final es Random Forest.</t>
+  </si>
+  <si>
+    <t>Experimiento_012_Proyecto_ML_Ensamble_Stacking.ipynb</t>
   </si>
 </sst>
 </file>
@@ -242,7 +680,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +690,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,8 +735,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -577,21 +1024,21 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="22.21875" customWidth="1"/>
-    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" customWidth="1"/>
+    <col min="3" max="3" width="72.109375" customWidth="1"/>
     <col min="4" max="4" width="10.77734375" customWidth="1"/>
     <col min="5" max="5" width="13.44140625" customWidth="1"/>
     <col min="6" max="6" width="15.21875" customWidth="1"/>
-    <col min="7" max="7" width="50.5546875" customWidth="1"/>
+    <col min="7" max="7" width="51.44140625" customWidth="1"/>
     <col min="8" max="8" width="60.44140625" customWidth="1"/>
-    <col min="9" max="9" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
@@ -602,7 +1049,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
@@ -620,7 +1067,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" ht="95.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -640,16 +1087,16 @@
         <v>44735</v>
       </c>
       <c r="F2" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -660,7 +1107,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4">
         <v>0.75609999999999999</v>
@@ -669,16 +1116,16 @@
         <v>44735</v>
       </c>
       <c r="F3" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="4" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -686,10 +1133,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D4" s="4">
         <v>0.63360000000000005</v>
@@ -698,100 +1145,301 @@
         <v>44736</v>
       </c>
       <c r="F4" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="3"/>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.63280000000000003</v>
+      </c>
+      <c r="E5" s="6">
+        <v>44737</v>
+      </c>
+      <c r="F5" s="3">
+        <v>22</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.63239999999999996</v>
+      </c>
+      <c r="E6" s="6">
+        <v>44737</v>
+      </c>
+      <c r="F6" s="3">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="3"/>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.69189999999999996</v>
+      </c>
+      <c r="E7" s="6">
+        <v>44737</v>
+      </c>
+      <c r="F7" s="3">
+        <v>22</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" ht="93.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="3"/>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0.7581</v>
+      </c>
+      <c r="E8" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F8" s="3">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" ht="90.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="3"/>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.68700000000000006</v>
+      </c>
+      <c r="E9" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F9" s="3">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="4" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="3"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F10" s="3">
+        <v>22</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="4" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="8"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="E11" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F11" s="3">
+        <v>22</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="199.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F12" s="3">
+        <v>22</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="197.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="E13" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F13" s="3">
+        <v>22</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="E14" s="6"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="6">
+        <v>44738</v>
+      </c>
+      <c r="F14" s="3">
+        <v>22</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">

</xml_diff>